<commit_message>
Arreglos de la version 1.4.7
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/Cierre.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/Cierre.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="15450"/>
+    <workbookView xWindow="0" yWindow="1656" windowWidth="28800" windowHeight="15456"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,7 +107,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,11 +182,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -196,23 +211,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,140 +515,148 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+      <selection activeCell="C3" sqref="C3:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A5" s="5" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="A16:B17"/>
     <mergeCell ref="C16:D17"/>
     <mergeCell ref="A10:B11"/>
@@ -644,14 +667,6 @@
     <mergeCell ref="A14:B15"/>
     <mergeCell ref="C14:D15"/>
     <mergeCell ref="A8:B9"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="0" scale="40" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios listos de Bodegaje e IVA
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/Cierre.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/Cierre.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtjarquinm\Documents\GitHub-Donovan\Empe-o\Empeño.WindowsForms\Empeños\ComprobantesIVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CC6B47-351A-4803-A1FB-7EA24EF50FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1656" windowWidth="28800" windowHeight="15456"/>
+    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$D$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$D$21</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>Monto Empeño:</t>
-  </si>
-  <si>
     <t>Monto Intereses:</t>
   </si>
   <si>
@@ -57,12 +55,24 @@
   </si>
   <si>
     <t>Empeños y Venta       D' SANTI</t>
+  </si>
+  <si>
+    <t>IVA:</t>
+  </si>
+  <si>
+    <t>Monto Avalúos:</t>
+  </si>
+  <si>
+    <t>Monto Empeños:</t>
+  </si>
+  <si>
+    <t>Monto Bodegajes:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,6 +203,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -205,6 +218,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,18 +238,6 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,147 +518,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" ht="104.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="1">
+      <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="11" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="1">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="11" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="34.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="3"/>
+    <row r="14" spans="1:4" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+    <row r="15" spans="1:4" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="1">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="32.5" customHeight="1" x14ac:dyDescent="1">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="1">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="30.5" customHeight="1" x14ac:dyDescent="1">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="24">
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:D11"/>
     <mergeCell ref="A3:B4"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="A6:B7"/>
@@ -657,16 +713,18 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="C14:D15"/>
     <mergeCell ref="A16:B17"/>
     <mergeCell ref="C16:D17"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
     <mergeCell ref="A12:B13"/>
-    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
     <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="A8:B9"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="0" scale="40" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>